<commit_message>
"Watch dog" works and small improvement to error logging
</commit_message>
<xml_diff>
--- a/Source/GoodSampleData.xlsx
+++ b/Source/GoodSampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin May\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin May\Desktop\TimingByToby\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="398">
   <si>
     <t>FirstName</t>
   </si>
@@ -1198,6 +1198,21 @@
   </si>
   <si>
     <t>Auctor Odio Consulting</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -1513,16 +1528,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H102" sqref="H102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="7" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1544,8 +1561,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1567,8 +1587,11 @@
       <c r="G2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1590,8 +1613,11 @@
       <c r="G3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1613,8 +1639,11 @@
       <c r="G4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1636,8 +1665,11 @@
       <c r="G5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1659,8 +1691,11 @@
       <c r="G6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1682,8 +1717,11 @@
       <c r="G7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1705,8 +1743,11 @@
       <c r="G8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1728,8 +1769,11 @@
       <c r="G9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1751,8 +1795,11 @@
       <c r="G10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1774,8 +1821,11 @@
       <c r="G11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1797,8 +1847,11 @@
       <c r="G12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1820,8 +1873,11 @@
       <c r="G13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1843,8 +1899,11 @@
       <c r="G14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1866,8 +1925,11 @@
       <c r="G15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1889,8 +1951,11 @@
       <c r="G16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1912,8 +1977,11 @@
       <c r="G17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1935,8 +2003,11 @@
       <c r="G18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1958,8 +2029,11 @@
       <c r="G19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1981,8 +2055,11 @@
       <c r="G20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2004,8 +2081,11 @@
       <c r="G21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -2027,8 +2107,11 @@
       <c r="G22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -2050,8 +2133,11 @@
       <c r="G23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -2073,8 +2159,11 @@
       <c r="G24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -2096,8 +2185,11 @@
       <c r="G25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -2119,8 +2211,11 @@
       <c r="G26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2142,8 +2237,11 @@
       <c r="G27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -2165,8 +2263,11 @@
       <c r="G28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2188,8 +2289,11 @@
       <c r="G29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -2211,8 +2315,11 @@
       <c r="G30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -2234,8 +2341,11 @@
       <c r="G31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>126</v>
       </c>
@@ -2257,8 +2367,11 @@
       <c r="G32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>130</v>
       </c>
@@ -2280,8 +2393,11 @@
       <c r="G33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>134</v>
       </c>
@@ -2303,8 +2419,11 @@
       <c r="G34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -2326,8 +2445,11 @@
       <c r="G35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>142</v>
       </c>
@@ -2349,8 +2471,11 @@
       <c r="G36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -2372,8 +2497,11 @@
       <c r="G37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -2395,8 +2523,11 @@
       <c r="G38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>154</v>
       </c>
@@ -2418,8 +2549,11 @@
       <c r="G39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>158</v>
       </c>
@@ -2441,8 +2575,11 @@
       <c r="G40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -2464,8 +2601,11 @@
       <c r="G41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -2487,8 +2627,11 @@
       <c r="G42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>170</v>
       </c>
@@ -2510,8 +2653,11 @@
       <c r="G43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>174</v>
       </c>
@@ -2533,8 +2679,11 @@
       <c r="G44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>178</v>
       </c>
@@ -2556,8 +2705,11 @@
       <c r="G45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>182</v>
       </c>
@@ -2579,8 +2731,11 @@
       <c r="G46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>186</v>
       </c>
@@ -2602,8 +2757,11 @@
       <c r="G47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>190</v>
       </c>
@@ -2625,8 +2783,11 @@
       <c r="G48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>194</v>
       </c>
@@ -2648,8 +2809,11 @@
       <c r="G49">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>198</v>
       </c>
@@ -2671,8 +2835,11 @@
       <c r="G50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>202</v>
       </c>
@@ -2694,8 +2861,11 @@
       <c r="G51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>206</v>
       </c>
@@ -2717,8 +2887,11 @@
       <c r="G52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>210</v>
       </c>
@@ -2740,8 +2913,11 @@
       <c r="G53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>214</v>
       </c>
@@ -2763,8 +2939,11 @@
       <c r="G54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>217</v>
       </c>
@@ -2786,8 +2965,11 @@
       <c r="G55">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>220</v>
       </c>
@@ -2809,8 +2991,11 @@
       <c r="G56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>224</v>
       </c>
@@ -2832,8 +3017,11 @@
       <c r="G57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>228</v>
       </c>
@@ -2855,8 +3043,11 @@
       <c r="G58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>232</v>
       </c>
@@ -2878,8 +3069,11 @@
       <c r="G59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>236</v>
       </c>
@@ -2901,8 +3095,11 @@
       <c r="G60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>240</v>
       </c>
@@ -2924,8 +3121,11 @@
       <c r="G61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>244</v>
       </c>
@@ -2947,8 +3147,11 @@
       <c r="G62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>248</v>
       </c>
@@ -2970,8 +3173,11 @@
       <c r="G63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>252</v>
       </c>
@@ -2993,8 +3199,11 @@
       <c r="G64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>256</v>
       </c>
@@ -3016,8 +3225,11 @@
       <c r="G65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H65" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>260</v>
       </c>
@@ -3039,8 +3251,11 @@
       <c r="G66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>264</v>
       </c>
@@ -3062,8 +3277,11 @@
       <c r="G67">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H67" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>268</v>
       </c>
@@ -3085,8 +3303,11 @@
       <c r="G68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>272</v>
       </c>
@@ -3108,8 +3329,11 @@
       <c r="G69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>276</v>
       </c>
@@ -3131,8 +3355,11 @@
       <c r="G70">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H70" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>280</v>
       </c>
@@ -3154,8 +3381,11 @@
       <c r="G71">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H71" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>284</v>
       </c>
@@ -3177,8 +3407,11 @@
       <c r="G72">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H72" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>288</v>
       </c>
@@ -3200,8 +3433,11 @@
       <c r="G73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>292</v>
       </c>
@@ -3223,8 +3459,11 @@
       <c r="G74">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>67</v>
       </c>
@@ -3246,8 +3485,11 @@
       <c r="G75">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>299</v>
       </c>
@@ -3269,8 +3511,11 @@
       <c r="G76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H76" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>302</v>
       </c>
@@ -3292,8 +3537,11 @@
       <c r="G77">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H77" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>306</v>
       </c>
@@ -3315,8 +3563,11 @@
       <c r="G78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H78" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>310</v>
       </c>
@@ -3338,8 +3589,11 @@
       <c r="G79">
         <v>4</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H79" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>314</v>
       </c>
@@ -3361,8 +3615,11 @@
       <c r="G80">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H80" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>318</v>
       </c>
@@ -3384,8 +3641,11 @@
       <c r="G81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H81" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>322</v>
       </c>
@@ -3407,8 +3667,11 @@
       <c r="G82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H82" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>324</v>
       </c>
@@ -3430,8 +3693,11 @@
       <c r="G83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H83" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>328</v>
       </c>
@@ -3453,8 +3719,11 @@
       <c r="G84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H84" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>332</v>
       </c>
@@ -3476,8 +3745,11 @@
       <c r="G85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H85" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>336</v>
       </c>
@@ -3499,8 +3771,11 @@
       <c r="G86">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H86" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>202</v>
       </c>
@@ -3522,8 +3797,11 @@
       <c r="G87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H87" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>343</v>
       </c>
@@ -3545,8 +3823,11 @@
       <c r="G88">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H88" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>347</v>
       </c>
@@ -3568,8 +3849,11 @@
       <c r="G89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H89" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>350</v>
       </c>
@@ -3591,8 +3875,11 @@
       <c r="G90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H90" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>253</v>
       </c>
@@ -3614,8 +3901,11 @@
       <c r="G91">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H91" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>356</v>
       </c>
@@ -3637,8 +3927,11 @@
       <c r="G92">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H92" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>360</v>
       </c>
@@ -3660,8 +3953,11 @@
       <c r="G93">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H93" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>276</v>
       </c>
@@ -3683,8 +3979,11 @@
       <c r="G94">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H94" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>367</v>
       </c>
@@ -3706,8 +4005,11 @@
       <c r="G95">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H95" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>370</v>
       </c>
@@ -3729,8 +4031,11 @@
       <c r="G96">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H96" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>374</v>
       </c>
@@ -3752,8 +4057,11 @@
       <c r="G97">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H97" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>378</v>
       </c>
@@ -3775,8 +4083,11 @@
       <c r="G98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>382</v>
       </c>
@@ -3798,8 +4109,11 @@
       <c r="G99">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H99" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>386</v>
       </c>
@@ -3821,8 +4135,11 @@
       <c r="G100">
         <v>4</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H100" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>389</v>
       </c>
@@ -3843,6 +4160,9 @@
       </c>
       <c r="G101">
         <v>3</v>
+      </c>
+      <c r="H101" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>